<commit_message>
determine RMSE for the teaching-lab slider
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Slider/TeachingLab_Slider_Crank/RMSE_Results/E/AngVel/f30_3RPM_csv/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Slider/TeachingLab_Slider_Crank/RMSE_Results/E/AngVel/f30_3RPM_csv/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teachinglab\Downloads\PMKS_Verification-master (1)\PMKS_Verification-master\Mechanisms\Four_Bar_Slider\TeachingLab_Slider_Crank\RMSE_Results\E\AngVel\f30_3RPM_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E9A47E-81AC-46D1-9FA1-1E1B47466CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAC470B-3799-45E4-8357-C830C5964661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="1620" windowWidth="21600" windowHeight="11295" xr2:uid="{6A19FCD9-925F-4E49-89A5-CC4040FB204F}"/>
+    <workbookView xWindow="3015" yWindow="1620" windowWidth="21600" windowHeight="11295" xr2:uid="{19EBF68B-2F46-4D3B-90C0-DF5C525AB5FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,13 +401,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5CC5CE-DFDE-4A07-86E8-F272D3D69964}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D422CC5-C9D3-4666-84EE-52748BA4A697}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>2.580090124932621E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>